<commit_message>
Update WTP Pain and Suffering values
Values taken from tables 10 and 11 in doi: 10.1007/s10198-022-01512-3

Dollar values are in AUD (2017)
</commit_message>
<xml_diff>
--- a/Data/WTPvaluesUncertainty.xlsx
+++ b/Data/WTPvaluesUncertainty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angus/Documents/AustralianFoodborneIllnessCosting/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u4859599\Documents\GitHub\FSANZ-ANU-Foodborne-Illness-Costing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E021C4-C5B1-BA4B-B61D-F69A46E5779D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D98A566-FAE8-4F14-9698-6B48AFCFB72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="2600" windowWidth="25440" windowHeight="14160" xr2:uid="{21524838-BEF9-CD4B-85A7-806F5D6A144B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{21524838-BEF9-CD4B-85A7-806F5D6A144B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,9 +137,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -177,7 +177,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -283,7 +283,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -425,7 +425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -436,12 +436,12 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -469,19 +469,19 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E2">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -489,19 +489,19 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -509,19 +509,19 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>17</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -532,16 +532,16 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -549,20 +549,19 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <f>964</f>
-        <v>964</v>
+        <v>1367</v>
       </c>
       <c r="D6">
-        <v>755</v>
+        <v>938</v>
       </c>
       <c r="E6">
-        <v>1100</v>
+        <v>1795</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -570,20 +569,19 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <f>344</f>
-        <v>344</v>
+        <v>575</v>
       </c>
       <c r="D7">
-        <v>124</v>
+        <v>272</v>
       </c>
       <c r="E7">
-        <v>506</v>
+        <v>877</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -591,20 +589,19 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <f>1166</f>
-        <v>1166</v>
+        <v>1412</v>
       </c>
       <c r="D8">
-        <v>1060</v>
+        <v>915</v>
       </c>
       <c r="E8">
-        <v>1241</v>
+        <v>1909</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -612,20 +609,19 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <f>605</f>
-        <v>605</v>
+        <v>531</v>
       </c>
       <c r="D9">
-        <v>461</v>
+        <v>156</v>
       </c>
       <c r="E9">
-        <v>714</v>
+        <v>907</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -633,20 +629,19 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <f>1620</f>
-        <v>1620</v>
+        <v>2195</v>
       </c>
       <c r="D10">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="E10">
-        <v>1637</v>
+        <v>2794</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -654,20 +649,19 @@
         <v>4</v>
       </c>
       <c r="C11">
-        <f>901</f>
-        <v>901</v>
+        <v>1025</v>
       </c>
       <c r="D11">
-        <v>778</v>
+        <v>630</v>
       </c>
       <c r="E11">
-        <v>993</v>
+        <v>1419</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -675,20 +669,19 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <f>1371</f>
-        <v>1371</v>
+        <v>1852</v>
       </c>
       <c r="D12">
-        <v>1291</v>
+        <v>1337</v>
       </c>
       <c r="E12">
-        <v>1426</v>
+        <v>2367</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -696,14 +689,13 @@
         <v>4</v>
       </c>
       <c r="C13">
-        <f>762</f>
-        <v>762</v>
+        <v>835</v>
       </c>
       <c r="D13">
-        <v>625</v>
+        <v>453</v>
       </c>
       <c r="E13">
-        <v>862</v>
+        <v>1217</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>

</xml_diff>